<commit_message>
final commit of work for Sensyne API for creating products and explanation of how I would build framework
</commit_message>
<xml_diff>
--- a/testSheet.xlsx
+++ b/testSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdulkadirmumin/qa-technical-test-master/SensyneHealth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C856807C-A22D-594D-9B30-53314E783724}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6E3BF3-C76A-1448-9560-5AE54A07369F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="67100" yWindow="500" windowWidth="28040" windowHeight="14860" xr2:uid="{EED7CB07-B4BB-214C-8262-FF5CDDE26C88}"/>
+    <workbookView xWindow="740" yWindow="2080" windowWidth="28040" windowHeight="14860" xr2:uid="{EED7CB07-B4BB-214C-8262-FF5CDDE26C88}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
   <si>
     <t>Description</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>Create product incorrect name and price</t>
-  </si>
-  <si>
-    <t>Create product incorrect URL</t>
   </si>
   <si>
     <t xml:space="preserve">Create a product with data in incorrect format for name </t>
@@ -111,9 +108,6 @@
     <t>Create a product with data in incorrect format for name and price</t>
   </si>
   <si>
-    <t>Create a product with data in correct format for name and price but incorrect URL</t>
-  </si>
-  <si>
     <t xml:space="preserve">"POST" request
 url = http://localhost:5000/v1/product
 Data: { name: "Harry"
@@ -126,12 +120,6 @@
 price: @!!} </t>
   </si>
   <si>
-    <t xml:space="preserve">"POST" request
-url = http://localhost:5000/v1/productt
-Data: { name: "John"
-price: 15.00} </t>
-  </si>
-  <si>
     <t>response body: Bad request, name cannot be string
 Response Code: 400</t>
   </si>
@@ -139,12 +127,12 @@
     <t>Pass</t>
   </si>
   <si>
+    <t>After running "GET" request for get list of products, the user can see that this product has been created. Therefore, the bug is that the API is getting the incorrect response code and response body as that post request has done what it is meant to do, which is to create a product. The verification process was done manually on web App</t>
+  </si>
+  <si>
     <t>response body: 
-Bad request, name cannot be string
+Bad request, request body is not valid JSON
 Response Code: 400</t>
-  </si>
-  <si>
-    <t>After running "GET" request for get list of products, the user can see that this product has been created. Therefore, the bug is that the API is getting the incorrect response code and response body as that post request has done what it is meant to do, which is to create a product. The verification process was done manually on web App</t>
   </si>
 </sst>
 </file>
@@ -575,10 +563,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076977DD-C99C-A24F-805A-13C1FB8A4549}">
-  <dimension ref="A1:H6"/>
+  <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,7 +617,7 @@
         <v>7</v>
       </c>
       <c r="D2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E2" s="4" t="s">
         <v>9</v>
@@ -641,7 +629,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -652,22 +640,22 @@
         <v>13</v>
       </c>
       <c r="C3" s="4" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="D3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="E3" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="F3" s="4" t="s">
         <v>26</v>
       </c>
-      <c r="F3" s="4" t="s">
-        <v>28</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>27</v>
+        <v>24</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A4" s="3">
         <v>3</v>
       </c>
@@ -675,10 +663,19 @@
         <v>14</v>
       </c>
       <c r="C4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="D4" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="E4" s="4" t="s">
         <v>23</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>24</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="102" x14ac:dyDescent="0.2">
@@ -689,24 +686,16 @@
         <v>15</v>
       </c>
       <c r="C5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D5" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="F5" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="G5" s="6" t="s">
         <v>24</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" ht="102" x14ac:dyDescent="0.2">
-      <c r="A6" s="3">
-        <v>5</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" s="4" t="s">
-        <v>22</v>
-      </c>
-      <c r="D6" s="4" t="s">
-        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
test sheet final update
</commit_message>
<xml_diff>
--- a/testSheet.xlsx
+++ b/testSheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/abdulkadirmumin/qa-technical-test-master/SensyneHealth/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF6E3BF3-C76A-1448-9560-5AE54A07369F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FF6EBE8-F4F1-A449-9D92-C86326F71026}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="740" yWindow="2080" windowWidth="28040" windowHeight="14860" xr2:uid="{EED7CB07-B4BB-214C-8262-FF5CDDE26C88}"/>
+    <workbookView xWindow="740" yWindow="2040" windowWidth="28040" windowHeight="14860" xr2:uid="{EED7CB07-B4BB-214C-8262-FF5CDDE26C88}"/>
   </bookViews>
   <sheets>
     <sheet name="Test Cases" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="27">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="30">
   <si>
     <t>Description</t>
   </si>
@@ -120,10 +120,6 @@
 price: @!!} </t>
   </si>
   <si>
-    <t>response body: Bad request, name cannot be string
-Response Code: 400</t>
-  </si>
-  <si>
     <t>Pass</t>
   </si>
   <si>
@@ -132,6 +128,23 @@
   <si>
     <t>response body: 
 Bad request, request body is not valid JSON
+Response Code: 400</t>
+  </si>
+  <si>
+    <t>response body: 
+Bad request, request body is not of type string
+Response Code: 400</t>
+  </si>
+  <si>
+    <t>response body: Bad request, not valid format for price
+Response Code: 400</t>
+  </si>
+  <si>
+    <t>response body: Bad request, name and price not valid format
+Response Code: 400</t>
+  </si>
+  <si>
+    <t>response body: Bad request, name not in format string
 Response Code: 400</t>
   </si>
 </sst>
@@ -565,8 +578,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{076977DD-C99C-A24F-805A-13C1FB8A4549}">
   <dimension ref="A1:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -629,7 +642,7 @@
         <v>8</v>
       </c>
       <c r="H2" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -646,13 +659,13 @@
         <v>18</v>
       </c>
       <c r="E3" s="4" t="s">
-        <v>23</v>
+        <v>29</v>
       </c>
       <c r="F3" s="4" t="s">
         <v>26</v>
       </c>
       <c r="G3" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="4" spans="1:8" ht="119" x14ac:dyDescent="0.2">
@@ -669,16 +682,16 @@
         <v>21</v>
       </c>
       <c r="E4" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="F4" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="F4" s="4" t="s">
-        <v>26</v>
-      </c>
-      <c r="G4" s="6" t="s">
-        <v>24</v>
-      </c>
     </row>
-    <row r="5" spans="1:8" ht="102" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" ht="119" x14ac:dyDescent="0.2">
       <c r="A5" s="3">
         <v>4</v>
       </c>
@@ -691,11 +704,14 @@
       <c r="D5" s="4" t="s">
         <v>22</v>
       </c>
+      <c r="E5" s="4" t="s">
+        <v>28</v>
+      </c>
       <c r="F5" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
   </sheetData>

</xml_diff>